<commit_message>
Full tile + level start
Initial temp designs for full floor plans (utilizing spacing) and full tileset as a single sheet.
</commit_message>
<xml_diff>
--- a/Level Design/Level_Design_Book.xlsx
+++ b/Level Design/Level_Design_Book.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Andre\GitHub\DungeonGoop\Level Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC60F111-9DF1-410A-8FD5-8C85AF37D2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D3B0883-E4FB-477A-B089-DB9595725C52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29295" yWindow="1500" windowWidth="27390" windowHeight="13395" activeTab="3" xr2:uid="{CA1DF132-283B-4423-BE0F-36DBE9B529A1}"/>
+    <workbookView xWindow="28860" yWindow="180" windowWidth="12225" windowHeight="15120" activeTab="3" xr2:uid="{CA1DF132-283B-4423-BE0F-36DBE9B529A1}"/>
   </bookViews>
   <sheets>
     <sheet name="Legend" sheetId="1" r:id="rId1"/>
@@ -460,7 +460,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="118">
+  <dxfs count="66">
     <dxf>
       <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
       <fill>
@@ -650,6 +650,25 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <numFmt numFmtId="178" formatCode=";;;\ &quot;~~~&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="175" formatCode=";;;\ &quot;Item&quot;"/>
       <fill>
         <patternFill>
@@ -749,13 +768,22 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="179" formatCode=";;;\ &quot;~~~&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
+      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
       <border>
@@ -770,20 +798,20 @@
     <dxf>
       <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
       <border>
@@ -796,22 +824,34 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
       <border>
@@ -824,34 +864,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
       <border>
@@ -864,10 +880,34 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dashDot">
+          <color auto="1"/>
+        </left>
+        <right style="dashDot">
+          <color auto="1"/>
+        </right>
+        <top style="dashDot">
+          <color auto="1"/>
+        </top>
+        <bottom style="dashDot">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF964B00"/>
         </patternFill>
       </fill>
       <border>
@@ -880,31 +920,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
+      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
       <fill>
         <patternFill>
           <bgColor rgb="FF964B00"/>
@@ -920,10 +936,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
+      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
       <border>
@@ -936,7 +952,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
+      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
@@ -952,10 +968,109 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
+      <numFmt numFmtId="175" formatCode=";;;\ &quot;Item&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dashDot">
+          <color auto="1"/>
+        </left>
+        <right style="dashDot">
+          <color auto="1"/>
+        </right>
+        <top style="dashDot">
+          <color auto="1"/>
+        </top>
+        <bottom style="dashDot">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="176" formatCode=";;;\ &quot;SPEC&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dashDot">
+          <color auto="1"/>
+        </left>
+        <right style="dashDot">
+          <color auto="1"/>
+        </right>
+        <top style="dashDot">
+          <color auto="1"/>
+        </top>
+        <bottom style="dashDot">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <numFmt numFmtId="177" formatCode=";;;\ &quot;TRIG&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF002060"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dashDot">
+          <color auto="1"/>
+        </left>
+        <right style="dashDot">
+          <color auto="1"/>
+        </right>
+        <top style="dashDot">
+          <color auto="1"/>
+        </top>
+        <bottom style="dashDot">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
       <border>
@@ -968,10 +1083,94 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="175" formatCode=";;;\ &quot;Item&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
+      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
       <border>
@@ -992,7 +1191,95 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="176" formatCode=";;;\ &quot;SPEC&quot;"/>
+      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF964B00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF964B00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="175" formatCode=";;;\ &quot;Item&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dashDot">
+          <color auto="1"/>
+        </left>
+        <right style="dashDot">
+          <color auto="1"/>
+        </right>
+        <top style="dashDot">
+          <color auto="1"/>
+        </top>
+        <bottom style="dashDot">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="179" formatCode=";;;\ &quot;Spec&quot;"/>
       <fill>
         <patternFill>
           <bgColor rgb="FF7030A0"/>
@@ -1043,37 +1330,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="179" formatCode=";;;\ &quot;~~~&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
+      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
         </patternFill>
       </fill>
       <border>
@@ -1086,22 +1346,22 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
+      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
         </patternFill>
       </fill>
       <border>
@@ -1114,22 +1374,34 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
+      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dotted">
+          <color auto="1"/>
+        </left>
+        <right style="dotted">
+          <color auto="1"/>
+        </right>
+        <top style="dotted">
+          <color auto="1"/>
+        </top>
+        <bottom style="dotted">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
       <border>
@@ -1142,34 +1414,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
         </patternFill>
       </fill>
       <border>
@@ -1182,10 +1430,34 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
+      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="dashDot">
+          <color auto="1"/>
+        </left>
+        <right style="dashDot">
+          <color auto="1"/>
+        </right>
+        <top style="dashDot">
+          <color auto="1"/>
+        </top>
+        <bottom style="dashDot">
+          <color auto="1"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF964B00"/>
         </patternFill>
       </fill>
       <border>
@@ -1198,31 +1470,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
+      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
       <fill>
         <patternFill>
           <bgColor rgb="FF964B00"/>
@@ -1238,10 +1486,10 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
+      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
         </patternFill>
       </fill>
       <border>
@@ -1254,7 +1502,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
+      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC000"/>
@@ -1270,10 +1518,13 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
+      <font>
+        <color theme="0"/>
+      </font>
+      <numFmt numFmtId="178" formatCode=";;;\ &quot;~~~&quot;"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
       <border>
@@ -1385,1194 +1636,13 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="179" formatCode=";;;\ &quot;~~~&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="30" formatCode="@"/>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
         </patternFill>
       </fill>
       <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode=";;;\ &quot;Item&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode=";;;\ &quot;SPEC&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="177" formatCode=";;;\ &quot;TRIG&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="179" formatCode=";;;\ &quot;~~~&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode=";;;\ &quot;Item&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode=";;;\ &quot;SPEC&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="177" formatCode=";;;\ &quot;TRIG&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="179" formatCode=";;;\ &quot;~~~&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode=";;;\ &quot;Item&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="176" formatCode=";;;\ &quot;SPEC&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="177" formatCode=";;;\ &quot;TRIG&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode=";;;\ &quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode=";;;&quot;&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode=";;;&quot;[[]]&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode=";;;&quot;Enemy&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dotted">
-          <color auto="1"/>
-        </left>
-        <right style="dotted">
-          <color auto="1"/>
-        </right>
-        <top style="dotted">
-          <color auto="1"/>
-        </top>
-        <bottom style="dotted">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="168" formatCode=";;;&quot;^^^&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="169" formatCode=";;;\ &quot;*/*&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="170" formatCode=";;;\ &quot;Stair&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="171" formatCode=";;;\ &quot;{     }&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="172" formatCode=";;;\ &quot;{XX}&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF964B00"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="173" formatCode=";;;\ &quot;NPC&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="174" formatCode=";;;\ &quot;_==_&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode=";;;\ &quot;Item&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="178" formatCode=";;;\ &quot;Spec&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <numFmt numFmtId="177" formatCode=";;;\ &quot;TRIG&quot;"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF002060"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="dashDot">
-          <color auto="1"/>
-        </left>
-        <right style="dashDot">
-          <color auto="1"/>
-        </right>
-        <top style="dashDot">
-          <color auto="1"/>
-        </top>
-        <bottom style="dashDot">
-          <color auto="1"/>
-        </bottom>
         <vertical/>
         <horizontal/>
       </border>
@@ -3490,59 +2560,59 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:ZZ1048576">
-    <cfRule type="containsText" dxfId="52" priority="8" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="65" priority="1" operator="containsText" text="&quot;">
+      <formula>NOT(ISERROR(SEARCH("""",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="2" operator="containsText" text="f1">
+      <formula>NOT(ISERROR(SEARCH("f1",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="63" priority="3" operator="containsText" text="f2">
+      <formula>NOT(ISERROR(SEARCH("f2",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="tr">
+      <formula>NOT(ISERROR(SEARCH("tr",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="61" priority="6" operator="containsText" text="sp">
+      <formula>NOT(ISERROR(SEARCH("sp",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="60" priority="7" operator="containsText" text="i">
+      <formula>NOT(ISERROR(SEARCH("i",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="59" priority="8" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="51" priority="2" operator="containsText" text="f1">
-      <formula>NOT(ISERROR(SEARCH("f1",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="50" priority="3" operator="containsText" text="f2">
-      <formula>NOT(ISERROR(SEARCH("f2",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="tr">
-      <formula>NOT(ISERROR(SEARCH("tr",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="48" priority="6" operator="containsText" text="sp">
-      <formula>NOT(ISERROR(SEARCH("sp",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="7" operator="containsText" text="i">
-      <formula>NOT(ISERROR(SEARCH("i",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="20" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="58" priority="20" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="21" operator="containsText" text="n">
+    <cfRule type="containsText" dxfId="57" priority="21" operator="containsText" text="n">
       <formula>NOT(ISERROR(SEARCH("n",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="22" operator="containsText" text="l">
+    <cfRule type="containsText" dxfId="56" priority="22" operator="containsText" text="l">
       <formula>NOT(ISERROR(SEARCH("l",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="23" operator="containsText" text="d">
+    <cfRule type="containsText" dxfId="55" priority="23" operator="containsText" text="d">
       <formula>NOT(ISERROR(SEARCH("d",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="24" operator="containsText" text="s">
+    <cfRule type="containsText" dxfId="54" priority="24" operator="containsText" text="s">
       <formula>NOT(ISERROR(SEARCH("s",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="25" operator="containsText" text="o">
+    <cfRule type="containsText" dxfId="53" priority="25" operator="containsText" text="o">
       <formula>NOT(ISERROR(SEARCH("o",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="26" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="52" priority="26" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH("t",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="39" priority="27" operator="containsText" text="e">
+    <cfRule type="containsText" dxfId="51" priority="27" operator="containsText" text="e">
       <formula>NOT(ISERROR(SEARCH("e",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="38" priority="28" operator="containsText" text="p">
+    <cfRule type="containsText" dxfId="50" priority="28" operator="containsText" text="p">
       <formula>NOT(ISERROR(SEARCH("p",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="29" operator="containsText" text="f">
+    <cfRule type="containsText" dxfId="49" priority="29" operator="containsText" text="f">
       <formula>NOT(ISERROR(SEARCH("f",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="36" priority="30" operator="containsText" text="x">
+    <cfRule type="containsText" dxfId="48" priority="30" operator="containsText" text="x">
       <formula>NOT(ISERROR(SEARCH("x",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="1" operator="containsText" text="&quot;">
-      <formula>NOT(ISERROR(SEARCH("""",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4047,46 +3117,46 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:ZZ1048576">
-    <cfRule type="containsText" dxfId="117" priority="1" operator="containsText" text="tr">
+    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="tr">
       <formula>NOT(ISERROR(SEARCH("tr",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="116" priority="2" operator="containsText" text="sp">
+    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="sp">
       <formula>NOT(ISERROR(SEARCH("sp",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="115" priority="3" operator="containsText" text="i">
+    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="i">
       <formula>NOT(ISERROR(SEARCH("i",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="114" priority="4" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="5" operator="containsText" text="n">
+    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="n">
       <formula>NOT(ISERROR(SEARCH("n",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="6" operator="containsText" text="l">
+    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="l">
       <formula>NOT(ISERROR(SEARCH("l",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="111" priority="7" operator="containsText" text="d">
+    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="d">
       <formula>NOT(ISERROR(SEARCH("d",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="110" priority="8" operator="containsText" text="s">
+    <cfRule type="containsText" dxfId="40" priority="8" operator="containsText" text="s">
       <formula>NOT(ISERROR(SEARCH("s",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="9" operator="containsText" text="o">
+    <cfRule type="containsText" dxfId="39" priority="9" operator="containsText" text="o">
       <formula>NOT(ISERROR(SEARCH("o",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="10" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="38" priority="10" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH("t",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="107" priority="11" operator="containsText" text="e">
+    <cfRule type="containsText" dxfId="37" priority="11" operator="containsText" text="e">
       <formula>NOT(ISERROR(SEARCH("e",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="106" priority="12" operator="containsText" text="p">
+    <cfRule type="containsText" dxfId="36" priority="12" operator="containsText" text="p">
       <formula>NOT(ISERROR(SEARCH("p",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="105" priority="13" operator="containsText" text="f">
+    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="f">
       <formula>NOT(ISERROR(SEARCH("f",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="104" priority="14" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="34" priority="14" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4592,52 +3662,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F1:ZZ1048576">
-    <cfRule type="containsText" dxfId="103" priority="1" operator="containsText" text="f1">
+    <cfRule type="containsText" dxfId="33" priority="1" operator="containsText" text="f1">
       <formula>NOT(ISERROR(SEARCH("f1",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="102" priority="2" operator="containsText" text="f2">
+    <cfRule type="containsText" dxfId="32" priority="2" operator="containsText" text="f2">
       <formula>NOT(ISERROR(SEARCH("f2",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="101" priority="3" operator="containsText" text="tr">
+    <cfRule type="containsText" dxfId="31" priority="3" operator="containsText" text="tr">
       <formula>NOT(ISERROR(SEARCH("tr",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="100" priority="4" operator="containsText" text="sp">
+    <cfRule type="containsText" dxfId="30" priority="4" operator="containsText" text="sp">
       <formula>NOT(ISERROR(SEARCH("sp",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="99" priority="5" operator="containsText" text="i">
+    <cfRule type="containsText" dxfId="29" priority="5" operator="containsText" text="i">
       <formula>NOT(ISERROR(SEARCH("i",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="6" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="28" priority="6" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="7" operator="containsText" text="n">
+    <cfRule type="containsText" dxfId="27" priority="7" operator="containsText" text="n">
       <formula>NOT(ISERROR(SEARCH("n",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="96" priority="8" operator="containsText" text="l">
+    <cfRule type="containsText" dxfId="26" priority="8" operator="containsText" text="l">
       <formula>NOT(ISERROR(SEARCH("l",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="95" priority="9" operator="containsText" text="d">
+    <cfRule type="containsText" dxfId="25" priority="9" operator="containsText" text="d">
       <formula>NOT(ISERROR(SEARCH("d",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="10" operator="containsText" text="s">
+    <cfRule type="containsText" dxfId="24" priority="10" operator="containsText" text="s">
       <formula>NOT(ISERROR(SEARCH("s",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="11" operator="containsText" text="o">
+    <cfRule type="containsText" dxfId="23" priority="11" operator="containsText" text="o">
       <formula>NOT(ISERROR(SEARCH("o",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="12" operator="containsText" text="t">
+    <cfRule type="containsText" dxfId="22" priority="12" operator="containsText" text="t">
       <formula>NOT(ISERROR(SEARCH("t",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="13" operator="containsText" text="e">
+    <cfRule type="containsText" dxfId="21" priority="13" operator="containsText" text="e">
       <formula>NOT(ISERROR(SEARCH("e",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="90" priority="14" operator="containsText" text="p">
+    <cfRule type="containsText" dxfId="20" priority="14" operator="containsText" text="p">
       <formula>NOT(ISERROR(SEARCH("p",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="89" priority="15" operator="containsText" text="f">
+    <cfRule type="containsText" dxfId="19" priority="15" operator="containsText" text="f">
       <formula>NOT(ISERROR(SEARCH("f",F1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="16" operator="containsText" text="w">
+    <cfRule type="containsText" dxfId="18" priority="16" operator="containsText" text="w">
       <formula>NOT(ISERROR(SEARCH("w",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4649,7 +3719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D649333-D32F-4043-A4F6-56DD9D642EED}">
   <dimension ref="A1:V43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AA24" sqref="AA24"/>
     </sheetView>
   </sheetViews>
@@ -5631,60 +4701,60 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F1:ZZ28 F40:ZZ1048576 F29:I39 K29:ZZ39">
-    <cfRule type="containsText" dxfId="34" priority="7" operator="containsText" text="w">
-      <formula>NOT(ISERROR(SEARCH("w",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="2" operator="containsText" text="f1">
-      <formula>NOT(ISERROR(SEARCH("f1",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="3" operator="containsText" text="f2">
-      <formula>NOT(ISERROR(SEARCH("f2",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="4" operator="containsText" text="tr">
-      <formula>NOT(ISERROR(SEARCH("tr",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="5" operator="containsText" text="sp">
-      <formula>NOT(ISERROR(SEARCH("sp",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="6" operator="containsText" text="i">
-      <formula>NOT(ISERROR(SEARCH("i",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="8" operator="containsText" text="b">
-      <formula>NOT(ISERROR(SEARCH("b",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="9" operator="containsText" text="n">
-      <formula>NOT(ISERROR(SEARCH("n",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="10" operator="containsText" text="l">
-      <formula>NOT(ISERROR(SEARCH("l",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="11" operator="containsText" text="d">
-      <formula>NOT(ISERROR(SEARCH("d",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="12" operator="containsText" text="s">
-      <formula>NOT(ISERROR(SEARCH("s",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="13" operator="containsText" text="o">
-      <formula>NOT(ISERROR(SEARCH("o",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="22" priority="14" operator="containsText" text="t">
-      <formula>NOT(ISERROR(SEARCH("t",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="15" operator="containsText" text="e">
-      <formula>NOT(ISERROR(SEARCH("e",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="16" operator="containsText" text="p">
-      <formula>NOT(ISERROR(SEARCH("p",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="17" operator="containsText" text="f">
-      <formula>NOT(ISERROR(SEARCH("f",F1)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="18" operator="containsText" text="x">
-      <formula>NOT(ISERROR(SEARCH("x",F1)))</formula>
-    </cfRule>
+  <conditionalFormatting sqref="F1:ZZ28 F29:I39 K29:ZZ39 F40:ZZ1048576">
     <cfRule type="containsText" dxfId="17" priority="1" operator="containsText" text="&quot;">
       <formula>NOT(ISERROR(SEARCH("""",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="2" operator="containsText" text="f1">
+      <formula>NOT(ISERROR(SEARCH("f1",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="3" operator="containsText" text="f2">
+      <formula>NOT(ISERROR(SEARCH("f2",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="14" priority="4" operator="containsText" text="tr">
+      <formula>NOT(ISERROR(SEARCH("tr",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="5" operator="containsText" text="sp">
+      <formula>NOT(ISERROR(SEARCH("sp",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="12" priority="6" operator="containsText" text="i">
+      <formula>NOT(ISERROR(SEARCH("i",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="11" priority="7" operator="containsText" text="w">
+      <formula>NOT(ISERROR(SEARCH("w",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="8" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="n">
+      <formula>NOT(ISERROR(SEARCH("n",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="l">
+      <formula>NOT(ISERROR(SEARCH("l",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="d">
+      <formula>NOT(ISERROR(SEARCH("d",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="12" operator="containsText" text="s">
+      <formula>NOT(ISERROR(SEARCH("s",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="13" operator="containsText" text="o">
+      <formula>NOT(ISERROR(SEARCH("o",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="14" operator="containsText" text="t">
+      <formula>NOT(ISERROR(SEARCH("t",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="15" operator="containsText" text="e">
+      <formula>NOT(ISERROR(SEARCH("e",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="16" operator="containsText" text="p">
+      <formula>NOT(ISERROR(SEARCH("p",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="17" operator="containsText" text="f">
+      <formula>NOT(ISERROR(SEARCH("f",F1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="18" operator="containsText" text="x">
+      <formula>NOT(ISERROR(SEARCH("x",F1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>